<commit_message>
[FEAT] Ordering columns and check empties
</commit_message>
<xml_diff>
--- a/Excel1.xlsx
+++ b/Excel1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerson Lima\Documents\projetos\compare_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC63539-8A52-40B0-8987-4C278E767E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2A6751-ADB8-4CC6-810F-60B9A1AD9161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5820" yWindow="-16200" windowWidth="13935" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Coluna A</t>
   </si>
@@ -45,15 +45,9 @@
     <t>Linha A4</t>
   </si>
   <si>
-    <t>Linha B2</t>
-  </si>
-  <si>
     <t>Linha C2</t>
   </si>
   <si>
-    <t>Linha B3</t>
-  </si>
-  <si>
     <t>Linha B4</t>
   </si>
   <si>
@@ -61,6 +55,9 @@
   </si>
   <si>
     <t>Linha C4</t>
+  </si>
+  <si>
+    <t>Linha BB</t>
   </si>
 </sst>
 </file>
@@ -386,8 +383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,29 +394,26 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -433,7 +427,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>